<commit_message>
cálculo da correlação entre Pger(MW) e q(m³/s) mudança da rotina de impressão das garantias físicas
</commit_message>
<xml_diff>
--- a/Resultados_Artigo.xlsx
+++ b/Resultados_Artigo.xlsx
@@ -478,13 +478,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K39" sqref="K39"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
imprimindo análises :correlação(p,q), frequencias e gfs
</commit_message>
<xml_diff>
--- a/Resultados_Artigo.xlsx
+++ b/Resultados_Artigo.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9330" windowHeight="10350" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9330" windowHeight="10350" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Garantia Física" sheetId="2" r:id="rId2"/>
+    <sheet name="Análises1" sheetId="3" r:id="rId3"/>
+    <sheet name="Análises" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="34">
   <si>
     <t>PCH1</t>
   </si>
@@ -76,12 +78,67 @@
   </si>
   <si>
     <t>mh_pph/</t>
+  </si>
+  <si>
+    <t>Corr(p,q)</t>
+  </si>
+  <si>
+    <t>GF_ma_prt(MWm)</t>
+  </si>
+  <si>
+    <t>GF_mh_prt(MWm)</t>
+  </si>
+  <si>
+    <t>GF_ma_pph(MWm)</t>
+  </si>
+  <si>
+    <t>GF_mh_pph(MWm)</t>
+  </si>
+  <si>
+    <t>frq_ma_prt(%)</t>
+  </si>
+  <si>
+    <t>frq_mh_prt(%)</t>
+  </si>
+  <si>
+    <t>frq_ma_pph(%)</t>
+  </si>
+  <si>
+    <t>frq_mh_pph(%)</t>
+  </si>
+  <si>
+    <t>Média(q)(m³/s)</t>
+  </si>
+  <si>
+    <t>Dvp(q) (m³/s)</t>
+  </si>
+  <si>
+    <t>Coluna1</t>
+  </si>
+  <si>
+    <t>Coluna4</t>
+  </si>
+  <si>
+    <t>Pinst/q_med</t>
+  </si>
+  <si>
+    <t>aumento freq em relação a ma_prt</t>
+  </si>
+  <si>
+    <t>diferença frq (ma_prt - mh_pph)</t>
+  </si>
+  <si>
+    <t>coef. Var</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,15 +177,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -136,12 +199,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -149,12 +292,117 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -165,6 +413,42 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="B2:R8" totalsRowShown="0">
+  <autoFilter ref="B2:R8"/>
+  <tableColumns count="17">
+    <tableColumn id="1" name="Coluna1"/>
+    <tableColumn id="2" name="GF_ma_prt(MWm)" dataDxfId="14"/>
+    <tableColumn id="3" name="GF_mh_prt(MWm)" dataDxfId="13"/>
+    <tableColumn id="4" name="GF_ma_pph(MWm)" dataDxfId="12"/>
+    <tableColumn id="5" name="GF_mh_pph(MWm)" dataDxfId="11"/>
+    <tableColumn id="15" name="Coluna4" dataDxfId="10">
+      <calculatedColumnFormula>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" name="frq_ma_prt(%)" dataDxfId="9"/>
+    <tableColumn id="7" name="frq_mh_prt(%)" dataDxfId="8"/>
+    <tableColumn id="8" name="frq_ma_pph(%)" dataDxfId="7"/>
+    <tableColumn id="9" name="frq_mh_pph(%)" dataDxfId="6"/>
+    <tableColumn id="14" name="diferença frq (ma_prt - mh_pph)" dataDxfId="5">
+      <calculatedColumnFormula>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" name="aumento freq em relação a ma_prt" dataCellStyle="Porcentagem">
+      <calculatedColumnFormula>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" name="Corr(p,q)" dataDxfId="4" dataCellStyle="Porcentagem"/>
+    <tableColumn id="11" name="Média(q)(m³/s)" dataDxfId="3"/>
+    <tableColumn id="12" name="Dvp(q) (m³/s)" dataDxfId="2"/>
+    <tableColumn id="13" name="coef. Var" dataDxfId="1">
+      <calculatedColumnFormula>P3/O3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" name="Pinst/q_med" dataDxfId="0">
+      <calculatedColumnFormula>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -478,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B44" sqref="B44:B47"/>
     </sheetView>
   </sheetViews>
@@ -1401,4 +1685,725 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:R8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="17.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8">
+        <v>13.231225698730265</v>
+      </c>
+      <c r="D3" s="9">
+        <v>11.094591700607745</v>
+      </c>
+      <c r="E3" s="9">
+        <v>13.205749018095807</v>
+      </c>
+      <c r="F3" s="9">
+        <v>12.577715014037262</v>
+      </c>
+      <c r="G3" s="10">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>0.65351068469300344</v>
+      </c>
+      <c r="H3" s="8">
+        <v>50.621890547263682</v>
+      </c>
+      <c r="I3" s="9">
+        <v>65.547263681592042</v>
+      </c>
+      <c r="J3" s="9">
+        <v>62.68656716417911</v>
+      </c>
+      <c r="K3" s="9">
+        <v>67.164179104477611</v>
+      </c>
+      <c r="L3" s="10">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>16.542288557213929</v>
+      </c>
+      <c r="M3" s="15">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.32678132678132676</v>
+      </c>
+      <c r="N3" s="14">
+        <v>0.98904367807142046</v>
+      </c>
+      <c r="O3" s="7">
+        <v>63.669527363184059</v>
+      </c>
+      <c r="P3" s="7">
+        <v>16.467658912631212</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" ref="Q3:Q8" si="0">P3/O3</f>
+        <v>0.25864270703151765</v>
+      </c>
+      <c r="R3" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>0.47118301709503574</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11">
+        <v>20.059682841461004</v>
+      </c>
+      <c r="D4" s="12">
+        <v>19.178923331627292</v>
+      </c>
+      <c r="E4" s="12">
+        <v>20.03269222279599</v>
+      </c>
+      <c r="F4" s="12">
+        <v>19.972205883675056</v>
+      </c>
+      <c r="G4" s="13">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>8.7476957785948883E-2</v>
+      </c>
+      <c r="H4" s="11">
+        <v>50.833333333333329</v>
+      </c>
+      <c r="I4" s="12">
+        <v>57.499999999999993</v>
+      </c>
+      <c r="J4" s="12">
+        <v>80</v>
+      </c>
+      <c r="K4" s="12">
+        <v>80</v>
+      </c>
+      <c r="L4" s="13">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>29.166666666666671</v>
+      </c>
+      <c r="M4" s="15">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.57377049180327888</v>
+      </c>
+      <c r="N4" s="14">
+        <v>0.96479768944466571</v>
+      </c>
+      <c r="O4" s="7">
+        <v>56.6293333333333</v>
+      </c>
+      <c r="P4" s="7">
+        <v>14.742286953656665</v>
+      </c>
+      <c r="Q4" s="7">
+        <f t="shared" si="0"/>
+        <v>0.26032951627525203</v>
+      </c>
+      <c r="R4" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>0.52976078357506151</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="23">
+        <v>19.720086789719694</v>
+      </c>
+      <c r="D5" s="24">
+        <v>15.360058312253914</v>
+      </c>
+      <c r="E5" s="24">
+        <v>19.716554155648566</v>
+      </c>
+      <c r="F5" s="24">
+        <v>18.715308839563463</v>
+      </c>
+      <c r="G5" s="25">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>1.0047779501562317</v>
+      </c>
+      <c r="H5" s="23">
+        <v>55.000000000000007</v>
+      </c>
+      <c r="I5" s="24">
+        <v>69.166666666666671</v>
+      </c>
+      <c r="J5" s="24">
+        <v>60</v>
+      </c>
+      <c r="K5" s="24">
+        <v>70</v>
+      </c>
+      <c r="L5" s="25">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>14.999999999999993</v>
+      </c>
+      <c r="M5" s="16">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.27272727272727254</v>
+      </c>
+      <c r="N5" s="17">
+        <v>0.71973877735744018</v>
+      </c>
+      <c r="O5" s="18">
+        <v>113.99833333333332</v>
+      </c>
+      <c r="P5" s="18">
+        <v>88.899945621335007</v>
+      </c>
+      <c r="Q5" s="18">
+        <f t="shared" si="0"/>
+        <v>0.7798354855012648</v>
+      </c>
+      <c r="R5" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>0.26316174213073296</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="23">
+        <v>20.238504878406172</v>
+      </c>
+      <c r="D6" s="24">
+        <v>17.954239269369797</v>
+      </c>
+      <c r="E6" s="24">
+        <v>20.216564407624432</v>
+      </c>
+      <c r="F6" s="24">
+        <v>19.874969322839991</v>
+      </c>
+      <c r="G6" s="25">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>0.36353555556618034</v>
+      </c>
+      <c r="H6" s="23">
+        <v>53.055555555555557</v>
+      </c>
+      <c r="I6" s="24">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="J6" s="24">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="K6" s="24">
+        <v>70</v>
+      </c>
+      <c r="L6" s="25">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>16.944444444444443</v>
+      </c>
+      <c r="M6" s="16">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.31937172774869105</v>
+      </c>
+      <c r="N6" s="17">
+        <v>0.73624561903173968</v>
+      </c>
+      <c r="O6" s="18">
+        <v>85.647861111111098</v>
+      </c>
+      <c r="P6" s="18">
+        <v>61.229738333714877</v>
+      </c>
+      <c r="Q6" s="18">
+        <f>P6/O6</f>
+        <v>0.71490096237524769</v>
+      </c>
+      <c r="R6" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>0.35027144415294803</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="11">
+        <v>20.718822778225721</v>
+      </c>
+      <c r="D7" s="12">
+        <v>17.178177408473612</v>
+      </c>
+      <c r="E7" s="12">
+        <v>20.710106717273078</v>
+      </c>
+      <c r="F7" s="12">
+        <v>18.044905164612725</v>
+      </c>
+      <c r="G7" s="13">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>2.6739176136129963</v>
+      </c>
+      <c r="H7" s="11">
+        <v>62.922705314009661</v>
+      </c>
+      <c r="I7" s="12">
+        <v>77.536231884057969</v>
+      </c>
+      <c r="J7" s="12">
+        <v>68.115942028985515</v>
+      </c>
+      <c r="K7" s="12">
+        <v>76.811594202898547</v>
+      </c>
+      <c r="L7" s="13">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>13.888888888888886</v>
+      </c>
+      <c r="M7" s="15">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.2207293666026871</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0.86751656727185267</v>
+      </c>
+      <c r="O7" s="7">
+        <v>162.54045893719805</v>
+      </c>
+      <c r="P7" s="7">
+        <v>32.834335087090935</v>
+      </c>
+      <c r="Q7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.20200715133810085</v>
+      </c>
+      <c r="R7" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>0.18456943087376984</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="20">
+        <v>4.8799029552645345</v>
+      </c>
+      <c r="D8" s="21">
+        <v>3.4855178510067275</v>
+      </c>
+      <c r="E8" s="21">
+        <v>4.8714961256406344</v>
+      </c>
+      <c r="F8" s="21">
+        <v>4.2789911505180562</v>
+      </c>
+      <c r="G8" s="22">
+        <f>Tabela1[[#This Row],[GF_ma_prt(MWm)]]-Tabela1[[#This Row],[GF_mh_pph(MWm)]]</f>
+        <v>0.60091180474647832</v>
+      </c>
+      <c r="H8" s="20">
+        <v>47.361111111111107</v>
+      </c>
+      <c r="I8" s="21">
+        <v>68.055555555555557</v>
+      </c>
+      <c r="J8" s="21">
+        <v>60</v>
+      </c>
+      <c r="K8" s="21">
+        <v>70</v>
+      </c>
+      <c r="L8" s="22">
+        <f>Tabela1[[#This Row],[frq_mh_pph(%)]]-Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>22.638888888888893</v>
+      </c>
+      <c r="M8" s="16">
+        <f>Tabela1[[#This Row],[diferença frq (ma_prt - mh_pph)]]/Tabela1[[#This Row],[frq_ma_prt(%)]]</f>
+        <v>0.47800586510263943</v>
+      </c>
+      <c r="N8" s="17">
+        <v>0.99928337802985567</v>
+      </c>
+      <c r="O8" s="18">
+        <v>4.6437222222222223</v>
+      </c>
+      <c r="P8" s="18">
+        <v>2.4133118376316212</v>
+      </c>
+      <c r="Q8" s="18">
+        <f t="shared" si="0"/>
+        <v>0.51969341018781845</v>
+      </c>
+      <c r="R8" s="7">
+        <f>$R$1/Tabela1[[#This Row],[Média(q)(m³/s)]]</f>
+        <v>6.460334741048249</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:M8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>13.231225698730265</v>
+      </c>
+      <c r="D3">
+        <v>11.094591700607745</v>
+      </c>
+      <c r="E3">
+        <v>13.205749018095807</v>
+      </c>
+      <c r="F3">
+        <v>12.577715014037262</v>
+      </c>
+      <c r="G3">
+        <v>50.621890547263682</v>
+      </c>
+      <c r="H3">
+        <v>65.547263681592042</v>
+      </c>
+      <c r="I3">
+        <v>62.68656716417911</v>
+      </c>
+      <c r="J3">
+        <v>67.164179104477611</v>
+      </c>
+      <c r="K3">
+        <v>0.98904367807142046</v>
+      </c>
+      <c r="L3">
+        <v>63.669527363184059</v>
+      </c>
+      <c r="M3">
+        <v>16.467658912631212</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>20.059682841461004</v>
+      </c>
+      <c r="D4">
+        <v>19.178923331627292</v>
+      </c>
+      <c r="E4">
+        <v>20.03269222279599</v>
+      </c>
+      <c r="F4">
+        <v>19.972205883675056</v>
+      </c>
+      <c r="G4">
+        <v>50.833333333333329</v>
+      </c>
+      <c r="H4">
+        <v>57.499999999999993</v>
+      </c>
+      <c r="I4">
+        <v>80</v>
+      </c>
+      <c r="J4">
+        <v>80</v>
+      </c>
+      <c r="K4">
+        <v>0.96479768944466571</v>
+      </c>
+      <c r="L4">
+        <v>56.6293333333333</v>
+      </c>
+      <c r="M4">
+        <v>14.742286953656665</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>19.720086789719694</v>
+      </c>
+      <c r="D5">
+        <v>15.360058312253914</v>
+      </c>
+      <c r="E5">
+        <v>19.716554155648566</v>
+      </c>
+      <c r="F5">
+        <v>18.715308839563463</v>
+      </c>
+      <c r="G5">
+        <v>55.000000000000007</v>
+      </c>
+      <c r="H5">
+        <v>69.166666666666671</v>
+      </c>
+      <c r="I5">
+        <v>60</v>
+      </c>
+      <c r="J5">
+        <v>70</v>
+      </c>
+      <c r="K5">
+        <v>0.71973877735744018</v>
+      </c>
+      <c r="L5">
+        <v>113.99833333333332</v>
+      </c>
+      <c r="M5">
+        <v>88.899945621335007</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>20.238504878406172</v>
+      </c>
+      <c r="D6">
+        <v>17.954239269369797</v>
+      </c>
+      <c r="E6">
+        <v>20.216564407624432</v>
+      </c>
+      <c r="F6">
+        <v>19.874969322839991</v>
+      </c>
+      <c r="G6">
+        <v>53.055555555555557</v>
+      </c>
+      <c r="H6">
+        <v>61.388888888888893</v>
+      </c>
+      <c r="I6">
+        <v>66.666666666666657</v>
+      </c>
+      <c r="J6">
+        <v>70</v>
+      </c>
+      <c r="K6">
+        <v>0.73624561903173968</v>
+      </c>
+      <c r="L6">
+        <v>85.647861111111098</v>
+      </c>
+      <c r="M6">
+        <v>61.229738333714877</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>20.718822778225721</v>
+      </c>
+      <c r="D7">
+        <v>17.178177408473612</v>
+      </c>
+      <c r="E7">
+        <v>20.710106717273078</v>
+      </c>
+      <c r="F7">
+        <v>18.044905164612725</v>
+      </c>
+      <c r="G7">
+        <v>62.922705314009661</v>
+      </c>
+      <c r="H7">
+        <v>77.536231884057969</v>
+      </c>
+      <c r="I7">
+        <v>68.115942028985515</v>
+      </c>
+      <c r="J7">
+        <v>76.811594202898547</v>
+      </c>
+      <c r="K7">
+        <v>0.86751656727185267</v>
+      </c>
+      <c r="L7">
+        <v>162.54045893719805</v>
+      </c>
+      <c r="M7">
+        <v>32.834335087090935</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>4.8799029552645345</v>
+      </c>
+      <c r="D8">
+        <v>3.4855178510067275</v>
+      </c>
+      <c r="E8">
+        <v>4.8714961256406344</v>
+      </c>
+      <c r="F8">
+        <v>4.2789911505180562</v>
+      </c>
+      <c r="G8">
+        <v>47.361111111111107</v>
+      </c>
+      <c r="H8">
+        <v>68.055555555555557</v>
+      </c>
+      <c r="I8">
+        <v>60</v>
+      </c>
+      <c r="J8">
+        <v>70</v>
+      </c>
+      <c r="K8">
+        <v>0.99928337802985567</v>
+      </c>
+      <c r="L8">
+        <v>4.6437222222222223</v>
+      </c>
+      <c r="M8">
+        <v>2.4133118376316212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>